<commit_message>
r and update excel
</commit_message>
<xml_diff>
--- a/docs/semiconductors/section1/topic3/assets/pa-Adjustable-Regulation-and-Project1.xlsx
+++ b/docs/semiconductors/section1/topic3/assets/pa-Adjustable-Regulation-and-Project1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\a-Computer-Engineering\Semiconductors-Private\g-Diode-Applications\c-Filtering-and-Regulation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83CA776D-5BD8-45AD-8CF8-0C287E37494B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E981138A-7B00-4BDE-B965-919D7EF85F61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="3" xr2:uid="{E80DF3CB-22C8-48CC-A275-866A023A71E1}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{E80DF3CB-22C8-48CC-A275-866A023A71E1}"/>
   </bookViews>
   <sheets>
     <sheet name="L-HW-AdjReg" sheetId="11" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="89">
   <si>
     <t>#Diodes</t>
   </si>
@@ -182,9 +182,6 @@
     <t>R4_max</t>
   </si>
   <si>
-    <t>1.33 (5%)</t>
-  </si>
-  <si>
     <t>Voverhead</t>
   </si>
   <si>
@@ -281,13 +278,34 @@
     <t>1550 (2%)</t>
   </si>
   <si>
-    <t>Choose R3 to be as close to R3_max. Closest real value = 1500 ohm</t>
-  </si>
-  <si>
     <t>0.81mA</t>
   </si>
   <si>
     <t>Choose a Rload to be R3+R4_min+R5 = 1500 + 0 + 1800 = 3300 Ohm.</t>
+  </si>
+  <si>
+    <t>R3+R4+R5</t>
+  </si>
+  <si>
+    <t>680 + 100 + 1800</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>(R3+R4+R5) in parallel with R1</t>
+  </si>
+  <si>
+    <t>Choose R3 to be between min and max but as close to R3_max as possible</t>
+  </si>
+  <si>
+    <t>Use 115 as it is more realistic in lab</t>
+  </si>
+  <si>
+    <t>Calculated value is a worst case approximation, and significantly different than measured</t>
+  </si>
+  <si>
+    <t>This is an approximation, R4 half way</t>
   </si>
 </sst>
 </file>
@@ -296,8 +314,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.00000"/>
-    <numFmt numFmtId="166" formatCode="0.0"/>
-    <numFmt numFmtId="167" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="0.0000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -346,7 +364,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -355,13 +373,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
@@ -370,16 +388,16 @@
     <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
@@ -409,6 +427,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -577,8 +596,8 @@
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>91787</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>618260</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>129020</xdr:rowOff>
     </xdr:to>
@@ -933,7 +952,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90CB45F1-6375-45DC-9E98-1629C0ECE700}">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A29" sqref="A29:XFD29"/>
     </sheetView>
   </sheetViews>
@@ -963,13 +982,13 @@
         <v>12</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.6">
@@ -1055,7 +1074,7 @@
         <v>680.00E-6</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.6">
@@ -1107,7 +1126,7 @@
         <v>50.00E-6</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.6">
@@ -1219,7 +1238,7 @@
         <v>7</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.6">
@@ -1316,7 +1335,7 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A24" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B24" s="1" t="str">
         <f>_xlfn.CONCAT(A22,"-",A11)</f>
@@ -1335,10 +1354,10 @@
         <v>10</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H24" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.6">
@@ -1347,7 +1366,7 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A26" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B26" s="1" t="str">
         <f>_xlfn.CONCAT("1.25/(",A11,"-1.25)")</f>
@@ -1363,12 +1382,12 @@
       </c>
       <c r="E26" s="10"/>
       <c r="H26" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A27" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B27" s="1" t="str">
         <f>_xlfn.CONCAT("1.25/(",A11,"-1.25)")</f>
@@ -1384,7 +1403,7 @@
       </c>
       <c r="E27" s="10"/>
       <c r="H27" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.6">
@@ -1407,7 +1426,7 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D29" s="14">
         <v>330</v>
@@ -1474,7 +1493,7 @@
         <v>1500</v>
       </c>
       <c r="H31" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.6">
@@ -1570,13 +1589,13 @@
         <v>12</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.6">
@@ -1662,7 +1681,7 @@
         <v>47.00E-6</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.6">
@@ -1759,7 +1778,7 @@
         <v>1</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.6">
@@ -1785,7 +1804,7 @@
         <v>2</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.6">
@@ -1811,7 +1830,7 @@
         <v>3</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.6">
@@ -1837,7 +1856,7 @@
         <v>5</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.6">
@@ -1863,7 +1882,7 @@
         <v>4</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1877,8 +1896,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9007B5E-E97B-4D6D-8B65-09795ACAA333}">
   <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView topLeftCell="A16" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
@@ -1907,13 +1926,13 @@
         <v>12</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.6">
@@ -1999,7 +2018,7 @@
         <v>47.00E-6</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.6">
@@ -2007,7 +2026,7 @@
         <v>25</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D10" s="18">
         <v>2.7</v>
@@ -2021,7 +2040,7 @@
         <v>29</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D11" s="1" t="str">
         <f>TEXT(1800,"##0.00E+0")</f>
@@ -2043,12 +2062,12 @@
         <v>50.00E-6</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B14" s="1" t="str">
         <f>_xlfn.CONCAT("1.25/(",A10,"-1.25)")</f>
@@ -2064,12 +2083,12 @@
       </c>
       <c r="E14" s="10"/>
       <c r="H14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B15" s="1" t="str">
         <f>_xlfn.CONCAT("1.25/(",A10,"-1.25)")</f>
@@ -2085,7 +2104,7 @@
       </c>
       <c r="E15" s="10"/>
       <c r="H15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.6">
@@ -2109,7 +2128,7 @@
         <v>12</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.6">
@@ -2125,7 +2144,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D18" s="17">
         <v>0</v>
@@ -2136,7 +2155,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A19" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B19" s="1" t="str">
         <f>_xlfn.CONCAT(A16,"-",A17)</f>
@@ -2156,7 +2175,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B20" s="1" t="str">
         <f>_xlfn.CONCAT(A16,"-",A18)</f>
@@ -2176,7 +2195,7 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A21" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D21" s="8">
         <v>1500</v>
@@ -2191,7 +2210,7 @@
         <v>1500</v>
       </c>
       <c r="H21" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.6">
@@ -2229,7 +2248,7 @@
         <v>14</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.6">
@@ -2338,7 +2357,7 @@
         <v>14</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.6">
@@ -2383,8 +2402,8 @@
       <c r="F31" s="2">
         <v>15</v>
       </c>
-      <c r="G31" s="2" t="s">
-        <v>47</v>
+      <c r="G31" s="2">
+        <v>0.28999999999999998</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.6">
@@ -2429,7 +2448,7 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A34" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B34" s="1" t="str">
         <f>_xlfn.CONCAT(A32,"-",A10)</f>
@@ -2445,7 +2464,7 @@
       </c>
       <c r="E34" s="5"/>
       <c r="H34" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.6">
@@ -2461,10 +2480,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C34BEEC2-5462-4B25-B586-99C42A00A461}">
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
@@ -2476,7 +2495,7 @@
     <col min="5" max="5" width="6.44921875" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="4.8984375" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="6.796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="61.19921875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="71.8984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.6">
@@ -2493,21 +2512,24 @@
         <v>12</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="2">
-        <v>120</v>
+      <c r="B2" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="D2" s="20">
+        <v>115</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>13</v>
@@ -2585,15 +2607,22 @@
         <v>47.00E-6</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A10" t="s">
-        <v>4</v>
+        <v>81</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>82</v>
       </c>
       <c r="D10" s="2">
-        <v>470</v>
+        <f>680+100+1800</f>
+        <v>2580</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>15</v>
@@ -2601,282 +2630,311 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A11" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="D11" s="20">
-        <v>4</v>
+        <v>83</v>
+      </c>
+      <c r="D11" s="2">
+        <v>470</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F11" s="2">
-        <v>5</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>67</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D12" s="2" t="str">
+        <f>TEXT(1/(1/D10+1/D11),"0.00")</f>
+        <v>397.57</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.6">
+      <c r="A13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="D13" s="20">
+        <v>4</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" s="2">
+        <v>5</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.6">
+      <c r="A14" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D12" s="2" t="str">
+      <c r="B14" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D14" s="2" t="str">
         <f>TEXT(1800,"##0.00E+0")</f>
         <v>1.80E+3</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E14" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.6">
-      <c r="A13" t="s">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.6">
+      <c r="A15" t="s">
         <v>43</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B15" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D13" s="2" t="str">
+      <c r="D15" s="2" t="str">
         <f>TEXT(0.00005,"##0.00E+0")</f>
         <v>50.00E-6</v>
       </c>
-      <c r="E13" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.6">
-      <c r="A15" t="s">
+      <c r="E15" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.6">
+      <c r="A17" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="1" t="str">
+      <c r="B17" s="1" t="str">
         <f>_xlfn.CONCAT(A2,"*sqrt(2)")</f>
         <v>Vrms_source*sqrt(2)</v>
       </c>
-      <c r="C15" s="1" t="str">
+      <c r="C17" s="1" t="str">
         <f>_xlfn.CONCAT(D2,"*sqrt(2)")</f>
-        <v>120*sqrt(2)</v>
-      </c>
-      <c r="D15" s="9" t="str">
+        <v>115*sqrt(2)</v>
+      </c>
+      <c r="D17" s="9" t="str">
         <f>TEXT(D2*SQRT(2),"0.00")</f>
-        <v>169.71</v>
-      </c>
-      <c r="E15" s="10" t="s">
+        <v>162.63</v>
+      </c>
+      <c r="E17" s="10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.6">
-      <c r="A16" t="s">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.6">
+      <c r="A18" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="1" t="str">
-        <f>_xlfn.CONCAT("(",A15,"/",A4,")/",A5)</f>
+      <c r="B18" s="1" t="str">
+        <f>_xlfn.CONCAT("(",A17,"/",A4,")/",A5)</f>
         <v>(Vp_source/Turns)/CTD</v>
       </c>
-      <c r="C16" s="1" t="str">
-        <f>_xlfn.CONCAT("(",D15,"/",D4,")/",D5)</f>
-        <v>(169.71/6)/2</v>
-      </c>
-      <c r="D16" s="11" t="str">
-        <f>TEXT((D15/D4)/D5,"0.00")</f>
-        <v>14.14</v>
-      </c>
-      <c r="E16" s="10" t="s">
+      <c r="C18" s="1" t="str">
+        <f>_xlfn.CONCAT("(",D17,"/",D4,")/",D5)</f>
+        <v>(162.63/6)/2</v>
+      </c>
+      <c r="D18" s="11" t="str">
+        <f>TEXT((D17/D4)/D5,"0.00")</f>
+        <v>13.55</v>
+      </c>
+      <c r="E18" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F18" s="2">
         <v>1</v>
       </c>
-      <c r="G16" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.6">
-      <c r="A17" t="s">
+      <c r="G18" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.6">
+      <c r="A19" t="s">
         <v>5</v>
       </c>
-      <c r="B17" s="1" t="str">
+      <c r="B19" s="1" t="str">
         <f>_xlfn.CONCAT(A6,"*",A7)</f>
         <v>Vdiode*#Diodes</v>
       </c>
-      <c r="C17" s="1" t="str">
+      <c r="C19" s="1" t="str">
         <f>_xlfn.CONCAT(D6,"*",D7)</f>
         <v>0.7*1</v>
       </c>
-      <c r="D17" s="9" t="str">
+      <c r="D19" s="9" t="str">
         <f>TEXT(D6*D7,"0.00")</f>
         <v>0.70</v>
       </c>
-      <c r="E17" s="10" t="s">
+      <c r="E19" s="10" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.6">
-      <c r="A18" t="s">
-        <v>20</v>
-      </c>
-      <c r="B18" s="1" t="str">
-        <f>_xlfn.CONCAT(A16,"-",A17)</f>
-        <v>Vp_secondary-Vdiodes</v>
-      </c>
-      <c r="C18" s="1" t="str">
-        <f>_xlfn.CONCAT(D16,"-",D17)</f>
-        <v>14.14-0.70</v>
-      </c>
-      <c r="D18" s="11" t="str">
-        <f>TEXT(D16-D17,"0.00")</f>
-        <v>13.44</v>
-      </c>
-      <c r="E18" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="F18" s="2">
-        <v>2</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.6">
-      <c r="A19" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19" s="1" t="str">
-        <f>_xlfn.CONCAT(A11,"/",A10)</f>
-        <v>Vreg/Rload</v>
-      </c>
-      <c r="C19" s="1" t="str">
-        <f>_xlfn.CONCAT(D11,"/",D10)</f>
-        <v>4/470</v>
-      </c>
-      <c r="D19" s="10" t="str">
-        <f>TEXT(D11/D10,"0.00000")</f>
-        <v>0.00851</v>
-      </c>
-      <c r="E19" s="10" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="1" t="str">
+        <f>_xlfn.CONCAT(A18,"-",A19)</f>
+        <v>Vp_secondary-Vdiodes</v>
+      </c>
+      <c r="C20" s="1" t="str">
+        <f>_xlfn.CONCAT(D18,"-",D19)</f>
+        <v>13.55-0.70</v>
+      </c>
+      <c r="D20" s="11" t="str">
+        <f>TEXT(D18-D19,"0.00")</f>
+        <v>12.85</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F20" s="2">
+        <v>2</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.6">
+      <c r="A21" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" s="1" t="str">
+        <f>_xlfn.CONCAT(A13,"/",A12)</f>
+        <v>Vreg/Rload</v>
+      </c>
+      <c r="C21" s="1" t="str">
+        <f>_xlfn.CONCAT(D13,"/",D12)</f>
+        <v>4/397.57</v>
+      </c>
+      <c r="D21" s="10" t="str">
+        <f>TEXT(D13/D12,"0.00000")</f>
+        <v>0.01006</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.6">
+      <c r="A22" t="s">
         <v>39</v>
       </c>
-      <c r="B20" s="1" t="str">
+      <c r="B22" s="1" t="str">
         <f>_xlfn.CONCAT("1/",A8)</f>
         <v>1/freq_rectifier</v>
       </c>
-      <c r="C20" s="1" t="str">
+      <c r="C22" s="1" t="str">
         <f>_xlfn.CONCAT("1/",D8)</f>
         <v>1/60</v>
       </c>
-      <c r="D20" s="10" t="str">
+      <c r="D22" s="10" t="str">
         <f>TEXT(1/D8,"0.00000")</f>
         <v>0.01667</v>
       </c>
-      <c r="E20" s="10" t="s">
+      <c r="E22" s="10" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.6">
-      <c r="A21" t="s">
-        <v>40</v>
-      </c>
-      <c r="B21" s="1" t="str">
-        <f>_xlfn.CONCAT("(",A19,"*",A20,")/",A9)</f>
-        <v>(I_load*Period_rectifier)/Crectifier</v>
-      </c>
-      <c r="C21" s="1" t="str">
-        <f>_xlfn.CONCAT("(",D19,"*",D20,")/",D9)</f>
-        <v>(0.00851*0.01667)/47.00E-6</v>
-      </c>
-      <c r="D21" s="13" t="str">
-        <f>TEXT((D19*D20)/(D9),"0.00")</f>
-        <v>3.02</v>
-      </c>
-      <c r="E21" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="F21" s="2">
-        <v>4</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.6">
-      <c r="A22" t="s">
-        <v>22</v>
-      </c>
-      <c r="B22" s="1" t="str">
-        <f>_xlfn.CONCAT(A18,"-",A21)</f>
-        <v>Vp_rectifier-Vrip_rectifier</v>
-      </c>
-      <c r="C22" s="1" t="str">
-        <f>_xlfn.CONCAT(D18,"-",D21)</f>
-        <v>13.44-3.02</v>
-      </c>
-      <c r="D22" s="9" t="str">
-        <f>TEXT(D18-D21,"0.00")</f>
-        <v>10.42</v>
-      </c>
-      <c r="E22" s="10" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="B23" s="1" t="str">
-        <f>_xlfn.CONCAT(A18,"-(",A21,"/2)")</f>
-        <v>Vp_rectifier-(Vrip_rectifier/2)</v>
+        <f>_xlfn.CONCAT("(",A21,"*",A22,")/",A9)</f>
+        <v>(I_load*Period_rectifier)/Crectifier</v>
       </c>
       <c r="C23" s="1" t="str">
-        <f>_xlfn.CONCAT(D18,"-(",D21,"/2)")</f>
-        <v>13.44-(3.02/2)</v>
-      </c>
-      <c r="D23" s="11" t="str">
-        <f>TEXT(D18-(D21/2),"0.00")</f>
-        <v>11.93</v>
+        <f>_xlfn.CONCAT("(",D21,"*",D22,")/",D9)</f>
+        <v>(0.01006*0.01667)/47.00E-6</v>
+      </c>
+      <c r="D23" s="13" t="str">
+        <f>TEXT((D21*D22)/(D9),"0.00")</f>
+        <v>3.57</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F23" s="2">
-        <v>3</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>65</v>
+        <v>4</v>
+      </c>
+      <c r="G23" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="H23" s="22" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A24" t="s">
-        <v>48</v>
+        <v>22</v>
       </c>
       <c r="B24" s="1" t="str">
-        <f>_xlfn.CONCAT(A22,"-",A11)</f>
+        <f>_xlfn.CONCAT(A20,"-",A23)</f>
+        <v>Vp_rectifier-Vrip_rectifier</v>
+      </c>
+      <c r="C24" s="1" t="str">
+        <f>_xlfn.CONCAT(D20,"-",D23)</f>
+        <v>12.85-3.57</v>
+      </c>
+      <c r="D24" s="9" t="str">
+        <f>TEXT(D20-D23,"0.00")</f>
+        <v>9.28</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.6">
+      <c r="A25" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" s="1" t="str">
+        <f>_xlfn.CONCAT(A20,"-(",A23,"/2)")</f>
+        <v>Vp_rectifier-(Vrip_rectifier/2)</v>
+      </c>
+      <c r="C25" s="1" t="str">
+        <f>_xlfn.CONCAT(D20,"-(",D23,"/2)")</f>
+        <v>12.85-(3.57/2)</v>
+      </c>
+      <c r="D25" s="11" t="str">
+        <f>TEXT(D20-(D23/2),"0.00")</f>
+        <v>11.07</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F25" s="2">
+        <v>3</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.6">
+      <c r="A26" t="s">
+        <v>47</v>
+      </c>
+      <c r="B26" s="1" t="str">
+        <f>_xlfn.CONCAT(A24,"-",A13)</f>
         <v>Vmin_rectifier-Vreg</v>
       </c>
-      <c r="C24" s="1" t="str">
-        <f>_xlfn.CONCAT(D22,"-",D11)</f>
-        <v>10.42-4</v>
-      </c>
-      <c r="D24" s="9" t="str">
-        <f>TEXT(D22-D11,"0.00")</f>
-        <v>6.42</v>
-      </c>
-      <c r="E24" s="10"/>
-      <c r="H24" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.6">
-      <c r="D25" s="10"/>
-      <c r="E25" s="10"/>
+      <c r="C26" s="1" t="str">
+        <f>_xlfn.CONCAT(D24,"-",D13)</f>
+        <v>9.28-4</v>
+      </c>
+      <c r="D26" s="9" t="str">
+        <f>TEXT(D24-D13,"0.00")</f>
+        <v>5.28</v>
+      </c>
+      <c r="E26" s="10"/>
+      <c r="H26" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.6">
+      <c r="D27" s="10"/>
+      <c r="E27" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>